<commit_message>
Updated MOVPE IKZ schema after merging of pull request
</commit_message>
<xml_diff>
--- a/movpe_IKZ_Ga2O3/Growth_GaO.xlsx
+++ b/movpe_IKZ_Ga2O3/Growth_GaO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="65">
   <si>
     <t xml:space="preserve"># start Header</t>
   </si>
@@ -94,75 +94,113 @@
     <t xml:space="preserve">Uniform MFC</t>
   </si>
   <si>
+    <t xml:space="preserve">Distance of showerhead from the susceptor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux of TEGa from MFC (Mass Flow Controller)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placeholder for format consistancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEGa partial pressure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEGa molar flux</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Flux of TEOS from MFC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Mass Flow Controller)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TEOS partial pressure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEOS molar flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxidant</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Flux of Oxygen from MFC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Mass Flow Controller)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">O2 molar flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># end Header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrate Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recipe Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T Shaft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T Filament</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T LayTec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrier Gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pushgas Valve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniform Valve</t>
+  </si>
+  <si>
     <t xml:space="preserve">Distance of Showerhead</t>
   </si>
   <si>
-    <t xml:space="preserve">Flux of Oxygen from TEGa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placeholder for format consistancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEGa partial pressure </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEGa molar flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flux of Oxygen from TEOS Mass Flow Controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEOS partial pressure </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEOS molar flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flux of Oxygen from MFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2 partial pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># end Header</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substrate Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recipe Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T Shaft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T Filament</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T LayTec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carrier Gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pushgas Valve</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uniform Valve</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bubbler Material</t>
   </si>
   <si>
@@ -193,13 +231,7 @@
     <t xml:space="preserve">Gas  Material</t>
   </si>
   <si>
-    <t xml:space="preserve">Flow from MFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas Partial Pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
+    <t xml:space="preserve">Comments</t>
   </si>
   <si>
     <t xml:space="preserve">20-158-G-1</t>
@@ -231,7 +263,7 @@
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -307,6 +339,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -559,7 +596,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -579,7 +616,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -603,7 +640,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -777,33 +814,32 @@
   </sheetPr>
   <dimension ref="A1:ALQ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M2" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AF17" activeCellId="0" sqref="AF17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="8.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="8" style="1" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="14" style="1" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="12.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="20" style="1" width="9.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="4" width="9.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="33" min="23" style="1" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1005" min="35" style="1" width="9.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="10.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="8.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="8" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="14" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="12.73"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="20" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="4" width="9.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="33" min="23" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1005" min="35" style="1" width="9.27"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -812,7 +848,7 @@
       <c r="G1" s="6"/>
       <c r="V1" s="7"/>
     </row>
-    <row r="2" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="8" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -821,7 +857,7 @@
       <c r="G2" s="9"/>
       <c r="V2" s="10"/>
     </row>
-    <row r="3" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="12" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
@@ -931,7 +967,7 @@
       <c r="AK3" s="16"/>
       <c r="AL3" s="16"/>
     </row>
-    <row r="4" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="21" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -973,7 +1009,7 @@
       <c r="AK4" s="20"/>
       <c r="AL4" s="20"/>
     </row>
-    <row r="5" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="14" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -1083,7 +1119,7 @@
       <c r="AK5" s="16"/>
       <c r="AL5" s="16"/>
     </row>
-    <row r="6" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="8" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1100,7 +1136,7 @@
       <c r="AK6" s="20"/>
       <c r="AL6" s="20"/>
     </row>
-    <row r="7" s="26" customFormat="true" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="26" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
         <v>16</v>
       </c>
@@ -1166,21 +1202,23 @@
       <c r="AE7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="AF7" s="23"/>
+      <c r="AF7" s="23" t="s">
+        <v>31</v>
+      </c>
       <c r="AG7" s="23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AH7" s="23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AI7" s="25"/>
       <c r="AJ7" s="16"/>
       <c r="AK7" s="16"/>
       <c r="AL7" s="16"/>
     </row>
-    <row r="8" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1197,106 +1235,106 @@
     </row>
     <row r="9" s="40" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K9" s="32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L9" s="32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M9" s="33" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="N9" s="34" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="O9" s="34" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P9" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="R9" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="S9" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="T9" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="U9" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="V9" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="W9" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="X9" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="R9" s="34" t="s">
+      <c r="Y9" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="S9" s="34" t="s">
+      <c r="Z9" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="AA9" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="U9" s="34" t="s">
+      <c r="AB9" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="V9" s="34" t="s">
+      <c r="AC9" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="W9" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="X9" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y9" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z9" s="35" t="s">
+      <c r="AD9" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE9" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF9" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG9" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="AA9" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB9" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC9" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD9" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE9" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF9" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG9" s="37" t="s">
+      <c r="AH9" s="36" t="s">
         <v>56</v>
-      </c>
-      <c r="AH9" s="36" t="s">
-        <v>57</v>
       </c>
       <c r="AI9" s="38" t="s">
         <v>58</v>
@@ -2322,15 +2360,9 @@
       <c r="P10" s="13" t="n">
         <v>1000</v>
       </c>
-      <c r="Q10" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="R10" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="S10" s="44" t="s">
-        <v>7</v>
-      </c>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
       <c r="T10" s="45" t="n">
         <v>20</v>
       </c>
@@ -3353,7 +3385,7 @@
       <c r="ALP10" s="39"/>
       <c r="ALQ10" s="39"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
@@ -3387,7 +3419,7 @@
       <c r="AH11" s="50"/>
       <c r="AI11" s="55"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="50"/>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
@@ -3421,7 +3453,7 @@
       <c r="AH12" s="50"/>
       <c r="AI12" s="55"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
@@ -3455,7 +3487,7 @@
       <c r="AH13" s="50"/>
       <c r="AI13" s="55"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>

</xml_diff>

<commit_message>
changes to bubbler and gas source in MOVPE IKZ
</commit_message>
<xml_diff>
--- a/movpe_IKZ_Ga2O3/Growth_GaO.xlsx
+++ b/movpe_IKZ_Ga2O3/Growth_GaO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
   <si>
     <t xml:space="preserve"># start Header</t>
   </si>
@@ -109,23 +109,7 @@
     <t xml:space="preserve">TEGa molar flux</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Flux of TEOS from MFC </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Mass Flow Controller)</t>
-    </r>
+    <t xml:space="preserve">Flux of TEOS from MFC (Mass Flow Controller)</t>
   </si>
   <si>
     <t xml:space="preserve">TEOS partial pressure </t>
@@ -137,23 +121,7 @@
     <t xml:space="preserve">Oxidant</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Flux of Oxygen from MFC </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Mass Flow Controller)</t>
-    </r>
+    <t xml:space="preserve">Flux of Oxygen from MFC (Mass Flow Controller)</t>
   </si>
   <si>
     <t xml:space="preserve">O2 molar flux</t>
@@ -204,31 +172,43 @@
     <t xml:space="preserve">Bubbler Material</t>
   </si>
   <si>
+    <t xml:space="preserve">Bubbler MFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bubbler Pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bubbler Dilution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bubbler Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bubbler Molar Flux</t>
+  </si>
+  <si>
     <t xml:space="preserve">MFC</t>
   </si>
   <si>
-    <t xml:space="preserve">Bubbler Pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bubbler Dilution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bubbler Temp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partial Pressure</t>
-  </si>
-  <si>
     <t xml:space="preserve">Molar Flux</t>
   </si>
   <si>
     <t xml:space="preserve">Gas  Material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas MFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas Molar Flux</t>
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
@@ -263,7 +243,7 @@
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -339,11 +319,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -596,7 +571,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -616,7 +591,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -632,15 +607,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -815,7 +790,7 @@
   <dimension ref="A1:ALQ14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M2" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF17" activeCellId="0" sqref="AF17"/>
+      <selection pane="topLeft" activeCell="AE17" activeCellId="0" sqref="AE17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1233,7 +1208,7 @@
       <c r="AK8" s="29"/>
       <c r="AL8" s="29"/>
     </row>
-    <row r="9" s="40" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="40" customFormat="true" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="30" t="s">
         <v>35</v>
       </c>
@@ -1304,7 +1279,7 @@
         <v>48</v>
       </c>
       <c r="X9" s="35" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="Y9" s="35" t="s">
         <v>50</v>
@@ -1325,19 +1300,19 @@
         <v>55</v>
       </c>
       <c r="AE9" s="35" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AF9" s="36" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AG9" s="37" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="AH9" s="36" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="AI9" s="38" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AJ9" s="16"/>
       <c r="AK9" s="16"/>
@@ -2312,13 +2287,13 @@
     </row>
     <row r="10" s="40" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D10" s="13" t="n">
         <v>210</v>
@@ -2352,7 +2327,7 @@
         <v>80</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="O10" s="44" t="n">
         <v>30</v>
@@ -2375,7 +2350,7 @@
         <v>0.00039285010895895</v>
       </c>
       <c r="W10" s="48" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="X10" s="44" t="n">
         <v>900</v>
@@ -2404,7 +2379,7 @@
         <v>2.03822378435889E-009</v>
       </c>
       <c r="AF10" s="48" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AG10" s="13" t="n">
         <v>500</v>

</xml_diff>

<commit_message>
extension of CZ IKZ parser
</commit_message>
<xml_diff>
--- a/movpe_IKZ_Ga2O3/Growth_GaO.xlsx
+++ b/movpe_IKZ_Ga2O3/Growth_GaO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="77">
   <si>
     <t xml:space="preserve"># start Header</t>
   </si>
@@ -76,6 +76,15 @@
     <t xml:space="preserve">#</t>
   </si>
   <si>
+    <t xml:space="preserve">History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The identifier of a step in the growth run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This index must be unique</t>
+  </si>
+  <si>
     <t xml:space="preserve">deposition time </t>
   </si>
   <si>
@@ -97,46 +106,10 @@
     <t xml:space="preserve">carrier gas type</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Pushgas </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Mass Flow Controller, MFC)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Uniform </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Mass Flow Controller, MFC)</t>
-    </r>
+    <t xml:space="preserve">Pushgas (Mass Flow Controller, MFC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniform (Mass Flow Controller, MFC)</t>
   </si>
   <si>
     <t xml:space="preserve">Distance of showerhead from the susceptor</t>
@@ -154,46 +127,10 @@
     <t xml:space="preserve">The gas flow of carrier gas (Mass Flow Controller, MFC)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The gas flow of concentrated precursor carried out from the bubbler </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Mass Flow Controller, MFC)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The gas flow of precursor injected into the chamber </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Mass Flow Controller, MFC)</t>
-    </r>
+    <t xml:space="preserve">The gas flow of concentrated precursor carried out from the bubbler (Mass Flow Controller, MFC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The gas flow of precursor injected into the chamber (Mass Flow Controller, MFC)</t>
   </si>
   <si>
     <t xml:space="preserve">Temperature of the precursor bubbler </t>
@@ -217,9 +154,18 @@
     <t xml:space="preserve">Substrate Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Previous Layer Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Recipe Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Step name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step Index</t>
+  </si>
+  <si>
     <t xml:space="preserve">Duration</t>
   </si>
   <si>
@@ -296,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve">200827_158_TEOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deposition</t>
   </si>
   <si>
     <t xml:space="preserve">TEGa </t>
@@ -403,12 +352,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -441,6 +384,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -548,7 +497,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -645,19 +594,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -697,7 +646,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -718,6 +667,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -893,50 +846,53 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:ALQ14"/>
+  <dimension ref="A1:ALT14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S22" activeCellId="0" sqref="S22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="14.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="16.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="8" style="1" width="9.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="14" style="1" width="9.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="12.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="12.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="9.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="4" width="9.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="23" style="1" width="9.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="11.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="33" min="28" style="1" width="9.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="11.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1005" min="35" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="16.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="11" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="17" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="11.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="12.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="25" min="25" style="4" width="9.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="29" min="26" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="11.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="36" min="31" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="11.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1008" min="38" style="1" width="9.27"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="V1" s="6"/>
+      <c r="Y1" s="6"/>
     </row>
     <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="V2" s="8"/>
+      <c r="Y2" s="8"/>
     </row>
-    <row r="3" s="10" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
@@ -947,54 +903,52 @@
         <v>3</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="O3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="P3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="Q3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="R3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="U3" s="10" t="s">
@@ -1003,22 +957,22 @@
       <c r="V3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="W3" s="10" t="s">
-        <v>3</v>
+      <c r="W3" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="X3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="Y3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AB3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="AC3" s="10" t="s">
@@ -1030,23 +984,32 @@
       <c r="AE3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AF3" s="13" t="s">
-        <v>3</v>
+      <c r="AF3" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="AG3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AH3" s="13" t="s">
+      <c r="AH3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AI3" s="11" t="s">
+      <c r="AI3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="14"/>
-      <c r="AL3" s="14"/>
+      <c r="AJ3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="14"/>
     </row>
-    <row r="4" s="19" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1059,12 +1022,12 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
@@ -1080,15 +1043,18 @@
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
       <c r="AE4" s="7"/>
-      <c r="AF4" s="16"/>
+      <c r="AF4" s="7"/>
       <c r="AG4" s="7"/>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="17"/>
-      <c r="AJ4" s="18"/>
-      <c r="AK4" s="18"/>
-      <c r="AL4" s="18"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="16"/>
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="17"/>
+      <c r="AM4" s="18"/>
+      <c r="AN4" s="18"/>
+      <c r="AO4" s="18"/>
     </row>
-    <row r="5" s="12" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
@@ -1099,343 +1065,365 @@
         <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="L5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="M5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="N5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="O5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="P5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="Q5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="R5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="T5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="U5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="V5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="W5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="12" t="s">
+      <c r="X5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="12" t="s">
+      <c r="Y5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="W5" s="12" t="s">
+      <c r="Z5" s="12" t="s">
         <v>7</v>
-      </c>
-      <c r="X5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z5" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="AA5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AB5" s="12" t="s">
+      <c r="AB5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AC5" s="12" t="s">
+      <c r="AD5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="AD5" s="12" t="s">
+      <c r="AG5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AE5" s="12" t="s">
+      <c r="AH5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AF5" s="21" t="s">
+      <c r="AI5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="AG5" s="12" t="s">
+      <c r="AJ5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AH5" s="21" t="s">
+      <c r="AK5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="AI5" s="20" t="s">
+      <c r="AL5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AJ5" s="14"/>
-      <c r="AK5" s="14"/>
-      <c r="AL5" s="14"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="14"/>
+      <c r="AO5" s="14"/>
     </row>
     <row r="6" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="AF6" s="16"/>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="18"/>
-      <c r="AK6" s="18"/>
-      <c r="AL6" s="18"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="AI6" s="16"/>
+      <c r="AK6" s="16"/>
+      <c r="AL6" s="15"/>
+      <c r="AM6" s="18"/>
+      <c r="AN6" s="18"/>
+      <c r="AO6" s="18"/>
     </row>
     <row r="7" s="27" customFormat="true" ht="106.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22" t="s">
+      <c r="C7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N7" s="22" t="s">
+      <c r="N7" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="O7" s="23" t="s">
         <v>28</v>
       </c>
       <c r="P7" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="23" t="s">
+      <c r="Q7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="R7" s="23" t="s">
+      <c r="R7" s="24" t="s">
         <v>31</v>
       </c>
       <c r="S7" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="T7" s="22" t="s">
+      <c r="T7" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22" t="s">
+      <c r="U7" s="23" t="s">
         <v>34</v>
       </c>
+      <c r="V7" s="23" t="s">
+        <v>35</v>
+      </c>
       <c r="W7" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="X7" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y7" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z7" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AA7" s="23" t="s">
+      <c r="AA7" s="24" t="s">
         <v>31</v>
       </c>
       <c r="AB7" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AC7" s="22" t="s">
+      <c r="AC7" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="AD7" s="22"/>
-      <c r="AE7" s="22" t="s">
+      <c r="AD7" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="AF7" s="24" t="s">
+      <c r="AE7" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AG7" s="24" t="s">
+      <c r="AF7" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="AH7" s="24"/>
-      <c r="AI7" s="25"/>
-      <c r="AJ7" s="26"/>
-      <c r="AK7" s="26"/>
-      <c r="AL7" s="26"/>
+      <c r="AG7" s="22"/>
+      <c r="AH7" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI7" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ7" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK7" s="24"/>
+      <c r="AL7" s="25"/>
+      <c r="AM7" s="26"/>
+      <c r="AN7" s="26"/>
+      <c r="AO7" s="26"/>
     </row>
     <row r="8" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="AF8" s="29"/>
-      <c r="AH8" s="29"/>
-      <c r="AI8" s="28"/>
-      <c r="AJ8" s="30"/>
-      <c r="AK8" s="30"/>
-      <c r="AL8" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="AI8" s="29"/>
+      <c r="AK8" s="29"/>
+      <c r="AL8" s="28"/>
+      <c r="AM8" s="30"/>
+      <c r="AN8" s="30"/>
+      <c r="AO8" s="30"/>
     </row>
     <row r="9" s="41" customFormat="true" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="31" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="E9" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="F9" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="31" t="s">
+      <c r="G9" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="H9" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="L9" s="33" t="s">
+      <c r="I9" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="34" t="s">
+      <c r="J9" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="N9" s="35" t="s">
+      <c r="K9" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="35" t="s">
+      <c r="L9" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="P9" s="35" t="s">
+      <c r="M9" s="31" t="s">
         <v>53</v>
       </c>
+      <c r="N9" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="P9" s="34" t="s">
+        <v>56</v>
+      </c>
       <c r="Q9" s="35" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="R9" s="35" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="S9" s="35" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="T9" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="U9" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="V9" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="W9" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="X9" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y9" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z9" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="U9" s="35" t="s">
+      <c r="AA9" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="V9" s="35" t="s">
+      <c r="AB9" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="W9" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="X9" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y9" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z9" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA9" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB9" s="36" t="s">
-        <v>56</v>
-      </c>
       <c r="AC9" s="36" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AD9" s="36" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="AE9" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF9" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG9" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH9" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="AI9" s="39" t="s">
+      <c r="AF9" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="AJ9" s="14"/>
-      <c r="AK9" s="14"/>
-      <c r="AL9" s="14"/>
-      <c r="AM9" s="40"/>
-      <c r="AN9" s="40"/>
-      <c r="AO9" s="40"/>
+      <c r="AG9" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH9" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI9" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ9" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK9" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL9" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM9" s="14"/>
+      <c r="AN9" s="14"/>
+      <c r="AO9" s="14"/>
       <c r="AP9" s="40"/>
       <c r="AQ9" s="40"/>
       <c r="AR9" s="40"/>
@@ -2400,114 +2388,123 @@
       <c r="ALO9" s="40"/>
       <c r="ALP9" s="40"/>
       <c r="ALQ9" s="40"/>
+      <c r="ALR9" s="40"/>
+      <c r="ALS9" s="40"/>
+      <c r="ALT9" s="40"/>
     </row>
     <row r="10" s="41" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="11" t="n">
+        <v>71</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" s="11" t="n">
         <v>210</v>
       </c>
-      <c r="E10" s="44" t="n">
+      <c r="H10" s="45" t="n">
         <v>840</v>
       </c>
-      <c r="F10" s="44" t="n">
+      <c r="I10" s="45" t="n">
         <v>815</v>
       </c>
-      <c r="G10" s="45" t="n">
+      <c r="J10" s="46" t="n">
         <v>804</v>
       </c>
-      <c r="H10" s="45" t="n">
+      <c r="K10" s="46" t="n">
         <v>25</v>
       </c>
-      <c r="I10" s="45" t="n">
+      <c r="L10" s="46" t="n">
         <v>500</v>
       </c>
-      <c r="J10" s="11" t="str">
+      <c r="M10" s="11" t="str">
         <f aca="false">[1]Overview!$I$10</f>
         <v>Argon</v>
       </c>
-      <c r="K10" s="46" t="n">
+      <c r="N10" s="47" t="n">
         <v>4900</v>
       </c>
-      <c r="L10" s="46" t="n">
+      <c r="O10" s="47" t="n">
         <v>1800</v>
       </c>
-      <c r="M10" s="46" t="n">
+      <c r="P10" s="47" t="n">
         <v>80</v>
       </c>
-      <c r="N10" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="O10" s="45" t="n">
+      <c r="Q10" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="R10" s="46" t="n">
         <v>30</v>
       </c>
-      <c r="P10" s="11" t="n">
+      <c r="S10" s="11" t="n">
         <v>1000</v>
       </c>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="46" t="n">
+      <c r="T10" s="46"/>
+      <c r="U10" s="46"/>
+      <c r="V10" s="46"/>
+      <c r="W10" s="47" t="n">
         <v>20</v>
       </c>
-      <c r="U10" s="47" t="n">
-        <f aca="false">1.333*10^(8.083-2162/(T10+273.15))</f>
+      <c r="X10" s="48" t="n">
+        <f aca="false">1.333*10^(8.083-2162/(W10+273.15))</f>
         <v>6.80402951697616</v>
       </c>
-      <c r="V10" s="48" t="n">
-        <f aca="false">(O10*U10)/((O10-U10)*22400)</f>
+      <c r="Y10" s="49" t="n">
+        <f aca="false">(R10*X10)/((R10-X10)*22400)</f>
         <v>0.00039285010895895</v>
       </c>
-      <c r="W10" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="X10" s="45" t="n">
+      <c r="Z10" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA10" s="46" t="n">
         <v>900</v>
       </c>
-      <c r="Y10" s="11" t="n">
+      <c r="AB10" s="11" t="n">
         <v>1000</v>
       </c>
-      <c r="Z10" s="45" t="n">
+      <c r="AC10" s="46" t="n">
         <v>1000</v>
       </c>
-      <c r="AA10" s="45" t="n">
+      <c r="AD10" s="46" t="n">
         <v>5</v>
       </c>
-      <c r="AB10" s="45" t="n">
+      <c r="AE10" s="46" t="n">
         <v>5</v>
       </c>
-      <c r="AC10" s="46" t="n">
+      <c r="AF10" s="47" t="n">
         <v>20</v>
       </c>
-      <c r="AD10" s="47" t="n">
-        <f aca="false">1.333*10^(8.742-2522/(AC10+273.15))</f>
+      <c r="AG10" s="48" t="n">
+        <f aca="false">1.333*10^(8.742-2522/(AF10+273.15))</f>
         <v>1.83537975333949</v>
       </c>
-      <c r="AE10" s="48" t="n">
-        <f aca="false">AD10*(AA10*AB10/(AA10+Z10))/Y10/22400</f>
+      <c r="AH10" s="49" t="n">
+        <f aca="false">AG10*(AD10*AE10/(AD10+AC10))/AB10/22400</f>
         <v>2.03822378435889E-009</v>
       </c>
-      <c r="AF10" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG10" s="11" t="n">
+      <c r="AI10" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ10" s="11" t="n">
         <v>500</v>
       </c>
-      <c r="AH10" s="11" t="n">
-        <f aca="false">AG10/22400</f>
+      <c r="AK10" s="11" t="n">
+        <f aca="false">AJ10/22400</f>
         <v>0.0223214285714286</v>
       </c>
-      <c r="AI10" s="50"/>
-      <c r="AJ10" s="40"/>
-      <c r="AK10" s="40"/>
-      <c r="AL10" s="40"/>
+      <c r="AL10" s="51"/>
       <c r="AM10" s="40"/>
       <c r="AN10" s="40"/>
       <c r="AO10" s="40"/>
@@ -3475,142 +3472,157 @@
       <c r="ALO10" s="40"/>
       <c r="ALP10" s="40"/>
       <c r="ALQ10" s="40"/>
+      <c r="ALR10" s="40"/>
+      <c r="ALS10" s="40"/>
+      <c r="ALT10" s="40"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="51"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="K11" s="53"/>
       <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="51"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
       <c r="Q11" s="52"/>
-      <c r="R11" s="52"/>
+      <c r="R11" s="53"/>
       <c r="S11" s="52"/>
       <c r="T11" s="53"/>
-      <c r="U11" s="54"/>
-      <c r="V11" s="55"/>
-      <c r="W11" s="55"/>
-      <c r="X11" s="52"/>
-      <c r="Y11" s="51"/>
-      <c r="Z11" s="52"/>
-      <c r="AA11" s="52"/>
+      <c r="U11" s="53"/>
+      <c r="V11" s="53"/>
+      <c r="W11" s="54"/>
+      <c r="X11" s="55"/>
+      <c r="Y11" s="56"/>
+      <c r="Z11" s="56"/>
+      <c r="AA11" s="53"/>
       <c r="AB11" s="52"/>
       <c r="AC11" s="53"/>
-      <c r="AD11" s="54"/>
-      <c r="AE11" s="55"/>
-      <c r="AF11" s="55"/>
-      <c r="AG11" s="51"/>
-      <c r="AH11" s="51"/>
+      <c r="AD11" s="53"/>
+      <c r="AE11" s="53"/>
+      <c r="AF11" s="54"/>
+      <c r="AG11" s="55"/>
+      <c r="AH11" s="56"/>
       <c r="AI11" s="56"/>
+      <c r="AJ11" s="52"/>
+      <c r="AK11" s="52"/>
+      <c r="AL11" s="57"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="51"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="K12" s="53"/>
       <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="51"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
       <c r="Q12" s="52"/>
-      <c r="R12" s="52"/>
+      <c r="R12" s="53"/>
       <c r="S12" s="52"/>
       <c r="T12" s="53"/>
-      <c r="U12" s="54"/>
-      <c r="V12" s="55"/>
-      <c r="W12" s="55"/>
-      <c r="X12" s="52"/>
-      <c r="Y12" s="51"/>
-      <c r="Z12" s="52"/>
-      <c r="AA12" s="52"/>
+      <c r="U12" s="53"/>
+      <c r="V12" s="53"/>
+      <c r="W12" s="54"/>
+      <c r="X12" s="55"/>
+      <c r="Y12" s="56"/>
+      <c r="Z12" s="56"/>
+      <c r="AA12" s="53"/>
       <c r="AB12" s="52"/>
       <c r="AC12" s="53"/>
-      <c r="AD12" s="54"/>
-      <c r="AE12" s="55"/>
-      <c r="AF12" s="55"/>
-      <c r="AG12" s="51"/>
-      <c r="AH12" s="51"/>
+      <c r="AD12" s="53"/>
+      <c r="AE12" s="53"/>
+      <c r="AF12" s="54"/>
+      <c r="AG12" s="55"/>
+      <c r="AH12" s="56"/>
       <c r="AI12" s="56"/>
+      <c r="AJ12" s="52"/>
+      <c r="AK12" s="52"/>
+      <c r="AL12" s="57"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="51"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="K13" s="53"/>
       <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="51"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="54"/>
       <c r="Q13" s="52"/>
-      <c r="R13" s="52"/>
+      <c r="R13" s="53"/>
       <c r="S13" s="52"/>
       <c r="T13" s="53"/>
-      <c r="U13" s="54"/>
-      <c r="V13" s="55"/>
-      <c r="W13" s="55"/>
-      <c r="X13" s="52"/>
-      <c r="Y13" s="51"/>
-      <c r="Z13" s="52"/>
-      <c r="AA13" s="52"/>
+      <c r="U13" s="53"/>
+      <c r="V13" s="53"/>
+      <c r="W13" s="54"/>
+      <c r="X13" s="55"/>
+      <c r="Y13" s="56"/>
+      <c r="Z13" s="56"/>
+      <c r="AA13" s="53"/>
       <c r="AB13" s="52"/>
       <c r="AC13" s="53"/>
-      <c r="AD13" s="54"/>
-      <c r="AE13" s="55"/>
-      <c r="AF13" s="55"/>
-      <c r="AG13" s="51"/>
-      <c r="AH13" s="51"/>
+      <c r="AD13" s="53"/>
+      <c r="AE13" s="53"/>
+      <c r="AF13" s="54"/>
+      <c r="AG13" s="55"/>
+      <c r="AH13" s="56"/>
       <c r="AI13" s="56"/>
+      <c r="AJ13" s="52"/>
+      <c r="AK13" s="52"/>
+      <c r="AL13" s="57"/>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="51"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="K14" s="53"/>
       <c r="L14" s="53"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="51"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
       <c r="Q14" s="52"/>
-      <c r="R14" s="52"/>
+      <c r="R14" s="53"/>
       <c r="S14" s="52"/>
       <c r="T14" s="53"/>
-      <c r="U14" s="54"/>
-      <c r="V14" s="55"/>
-      <c r="W14" s="55"/>
-      <c r="X14" s="52"/>
-      <c r="Y14" s="51"/>
-      <c r="Z14" s="52"/>
-      <c r="AA14" s="52"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="53"/>
+      <c r="W14" s="54"/>
+      <c r="X14" s="55"/>
+      <c r="Y14" s="56"/>
+      <c r="Z14" s="56"/>
+      <c r="AA14" s="53"/>
       <c r="AB14" s="52"/>
       <c r="AC14" s="53"/>
-      <c r="AD14" s="54"/>
-      <c r="AE14" s="55"/>
-      <c r="AF14" s="55"/>
-      <c r="AG14" s="51"/>
-      <c r="AH14" s="51"/>
+      <c r="AD14" s="53"/>
+      <c r="AE14" s="53"/>
+      <c r="AF14" s="54"/>
+      <c r="AG14" s="55"/>
+      <c r="AH14" s="56"/>
       <c r="AI14" s="56"/>
+      <c r="AJ14" s="52"/>
+      <c r="AK14" s="52"/>
+      <c r="AL14" s="57"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added somne classes to MOVPE IKY plugin
</commit_message>
<xml_diff>
--- a/movpe_IKZ_Ga2O3/Growth_GaO.xlsx
+++ b/movpe_IKZ_Ga2O3/Growth_GaO.xlsx
@@ -223,7 +223,7 @@
     <t xml:space="preserve">Bubbler Molar Flux</t>
   </si>
   <si>
-    <t xml:space="preserve">Gas  Material</t>
+    <t xml:space="preserve">Gas Material</t>
   </si>
   <si>
     <t xml:space="preserve">Gas MFC</t>
@@ -267,7 +267,7 @@
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -385,12 +385,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -497,7 +491,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -667,10 +661,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -848,8 +838,8 @@
   </sheetPr>
   <dimension ref="A1:ALT14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI9" activeCellId="0" sqref="AI9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2399,102 +2389,102 @@
       <c r="B10" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="44" t="n">
+      <c r="F10" s="43" t="n">
         <v>8</v>
       </c>
       <c r="G10" s="11" t="n">
         <v>210</v>
       </c>
-      <c r="H10" s="45" t="n">
+      <c r="H10" s="44" t="n">
         <v>840</v>
       </c>
-      <c r="I10" s="45" t="n">
+      <c r="I10" s="44" t="n">
         <v>815</v>
       </c>
-      <c r="J10" s="46" t="n">
+      <c r="J10" s="45" t="n">
         <v>804</v>
       </c>
-      <c r="K10" s="46" t="n">
+      <c r="K10" s="45" t="n">
         <v>25</v>
       </c>
-      <c r="L10" s="46" t="n">
+      <c r="L10" s="45" t="n">
         <v>500</v>
       </c>
       <c r="M10" s="11" t="str">
         <f aca="false">[1]Overview!$I$10</f>
         <v>Argon</v>
       </c>
-      <c r="N10" s="47" t="n">
+      <c r="N10" s="46" t="n">
         <v>4900</v>
       </c>
-      <c r="O10" s="47" t="n">
+      <c r="O10" s="46" t="n">
         <v>1800</v>
       </c>
-      <c r="P10" s="47" t="n">
+      <c r="P10" s="46" t="n">
         <v>80</v>
       </c>
       <c r="Q10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="R10" s="46" t="n">
+      <c r="R10" s="45" t="n">
         <v>30</v>
       </c>
       <c r="S10" s="11" t="n">
         <v>1000</v>
       </c>
-      <c r="T10" s="46"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="46"/>
-      <c r="W10" s="47" t="n">
+      <c r="T10" s="45"/>
+      <c r="U10" s="45"/>
+      <c r="V10" s="45"/>
+      <c r="W10" s="46" t="n">
         <v>20</v>
       </c>
-      <c r="X10" s="48" t="n">
+      <c r="X10" s="47" t="n">
         <f aca="false">1.333*10^(8.083-2162/(W10+273.15))</f>
         <v>6.80402951697616</v>
       </c>
-      <c r="Y10" s="49" t="n">
+      <c r="Y10" s="48" t="n">
         <f aca="false">(R10*X10)/((R10-X10)*22400)</f>
         <v>0.00039285010895895</v>
       </c>
-      <c r="Z10" s="50" t="s">
+      <c r="Z10" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="AA10" s="46" t="n">
+      <c r="AA10" s="45" t="n">
         <v>900</v>
       </c>
       <c r="AB10" s="11" t="n">
         <v>1000</v>
       </c>
-      <c r="AC10" s="46" t="n">
+      <c r="AC10" s="45" t="n">
         <v>1000</v>
       </c>
-      <c r="AD10" s="46" t="n">
+      <c r="AD10" s="45" t="n">
         <v>5</v>
       </c>
-      <c r="AE10" s="46" t="n">
+      <c r="AE10" s="45" t="n">
         <v>5</v>
       </c>
-      <c r="AF10" s="47" t="n">
+      <c r="AF10" s="46" t="n">
         <v>20</v>
       </c>
-      <c r="AG10" s="48" t="n">
+      <c r="AG10" s="47" t="n">
         <f aca="false">1.333*10^(8.742-2522/(AF10+273.15))</f>
         <v>1.83537975333949</v>
       </c>
-      <c r="AH10" s="49" t="n">
+      <c r="AH10" s="48" t="n">
         <f aca="false">AG10*(AD10*AE10/(AD10+AC10))/AB10/22400</f>
         <v>2.03822378435889E-009</v>
       </c>
-      <c r="AI10" s="50" t="s">
+      <c r="AI10" s="49" t="s">
         <v>76</v>
       </c>
       <c r="AJ10" s="11" t="n">
@@ -2504,7 +2494,7 @@
         <f aca="false">AJ10/22400</f>
         <v>0.0223214285714286</v>
       </c>
-      <c r="AL10" s="51"/>
+      <c r="AL10" s="50"/>
       <c r="AM10" s="40"/>
       <c r="AN10" s="40"/>
       <c r="AO10" s="40"/>
@@ -3477,152 +3467,152 @@
       <c r="ALT10" s="40"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="54"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="53"/>
-      <c r="S11" s="52"/>
-      <c r="T11" s="53"/>
-      <c r="U11" s="53"/>
-      <c r="V11" s="53"/>
-      <c r="W11" s="54"/>
-      <c r="X11" s="55"/>
-      <c r="Y11" s="56"/>
-      <c r="Z11" s="56"/>
-      <c r="AA11" s="53"/>
-      <c r="AB11" s="52"/>
-      <c r="AC11" s="53"/>
-      <c r="AD11" s="53"/>
-      <c r="AE11" s="53"/>
-      <c r="AF11" s="54"/>
-      <c r="AG11" s="55"/>
-      <c r="AH11" s="56"/>
-      <c r="AI11" s="56"/>
-      <c r="AJ11" s="52"/>
-      <c r="AK11" s="52"/>
-      <c r="AL11" s="57"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="52"/>
+      <c r="U11" s="52"/>
+      <c r="V11" s="52"/>
+      <c r="W11" s="53"/>
+      <c r="X11" s="54"/>
+      <c r="Y11" s="55"/>
+      <c r="Z11" s="55"/>
+      <c r="AA11" s="52"/>
+      <c r="AB11" s="51"/>
+      <c r="AC11" s="52"/>
+      <c r="AD11" s="52"/>
+      <c r="AE11" s="52"/>
+      <c r="AF11" s="53"/>
+      <c r="AG11" s="54"/>
+      <c r="AH11" s="55"/>
+      <c r="AI11" s="55"/>
+      <c r="AJ11" s="51"/>
+      <c r="AK11" s="51"/>
+      <c r="AL11" s="56"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="52"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="54"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="53"/>
-      <c r="U12" s="53"/>
-      <c r="V12" s="53"/>
-      <c r="W12" s="54"/>
-      <c r="X12" s="55"/>
-      <c r="Y12" s="56"/>
-      <c r="Z12" s="56"/>
-      <c r="AA12" s="53"/>
-      <c r="AB12" s="52"/>
-      <c r="AC12" s="53"/>
-      <c r="AD12" s="53"/>
-      <c r="AE12" s="53"/>
-      <c r="AF12" s="54"/>
-      <c r="AG12" s="55"/>
-      <c r="AH12" s="56"/>
-      <c r="AI12" s="56"/>
-      <c r="AJ12" s="52"/>
-      <c r="AK12" s="52"/>
-      <c r="AL12" s="57"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="51"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="52"/>
+      <c r="U12" s="52"/>
+      <c r="V12" s="52"/>
+      <c r="W12" s="53"/>
+      <c r="X12" s="54"/>
+      <c r="Y12" s="55"/>
+      <c r="Z12" s="55"/>
+      <c r="AA12" s="52"/>
+      <c r="AB12" s="51"/>
+      <c r="AC12" s="52"/>
+      <c r="AD12" s="52"/>
+      <c r="AE12" s="52"/>
+      <c r="AF12" s="53"/>
+      <c r="AG12" s="54"/>
+      <c r="AH12" s="55"/>
+      <c r="AI12" s="55"/>
+      <c r="AJ12" s="51"/>
+      <c r="AK12" s="51"/>
+      <c r="AL12" s="56"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="52"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="52"/>
-      <c r="T13" s="53"/>
-      <c r="U13" s="53"/>
-      <c r="V13" s="53"/>
-      <c r="W13" s="54"/>
-      <c r="X13" s="55"/>
-      <c r="Y13" s="56"/>
-      <c r="Z13" s="56"/>
-      <c r="AA13" s="53"/>
-      <c r="AB13" s="52"/>
-      <c r="AC13" s="53"/>
-      <c r="AD13" s="53"/>
-      <c r="AE13" s="53"/>
-      <c r="AF13" s="54"/>
-      <c r="AG13" s="55"/>
-      <c r="AH13" s="56"/>
-      <c r="AI13" s="56"/>
-      <c r="AJ13" s="52"/>
-      <c r="AK13" s="52"/>
-      <c r="AL13" s="57"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="51"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="52"/>
+      <c r="U13" s="52"/>
+      <c r="V13" s="52"/>
+      <c r="W13" s="53"/>
+      <c r="X13" s="54"/>
+      <c r="Y13" s="55"/>
+      <c r="Z13" s="55"/>
+      <c r="AA13" s="52"/>
+      <c r="AB13" s="51"/>
+      <c r="AC13" s="52"/>
+      <c r="AD13" s="52"/>
+      <c r="AE13" s="52"/>
+      <c r="AF13" s="53"/>
+      <c r="AG13" s="54"/>
+      <c r="AH13" s="55"/>
+      <c r="AI13" s="55"/>
+      <c r="AJ13" s="51"/>
+      <c r="AK13" s="51"/>
+      <c r="AL13" s="56"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="53"/>
-      <c r="S14" s="52"/>
-      <c r="T14" s="53"/>
-      <c r="U14" s="53"/>
-      <c r="V14" s="53"/>
-      <c r="W14" s="54"/>
-      <c r="X14" s="55"/>
-      <c r="Y14" s="56"/>
-      <c r="Z14" s="56"/>
-      <c r="AA14" s="53"/>
-      <c r="AB14" s="52"/>
-      <c r="AC14" s="53"/>
-      <c r="AD14" s="53"/>
-      <c r="AE14" s="53"/>
-      <c r="AF14" s="54"/>
-      <c r="AG14" s="55"/>
-      <c r="AH14" s="56"/>
-      <c r="AI14" s="56"/>
-      <c r="AJ14" s="52"/>
-      <c r="AK14" s="52"/>
-      <c r="AL14" s="57"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="53"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="52"/>
+      <c r="V14" s="52"/>
+      <c r="W14" s="53"/>
+      <c r="X14" s="54"/>
+      <c r="Y14" s="55"/>
+      <c r="Z14" s="55"/>
+      <c r="AA14" s="52"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="52"/>
+      <c r="AD14" s="52"/>
+      <c r="AE14" s="52"/>
+      <c r="AF14" s="53"/>
+      <c r="AG14" s="54"/>
+      <c r="AH14" s="55"/>
+      <c r="AI14" s="55"/>
+      <c r="AJ14" s="51"/>
+      <c r="AK14" s="51"/>
+      <c r="AL14" s="56"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>